<commit_message>
views annualization calculations removed
</commit_message>
<xml_diff>
--- a/Data/sample_portfolio2_views.xlsx
+++ b/Data/sample_portfolio2_views.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapam\Documents\Git\entropy-poolin\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9959CBB5-CA23-444C-A798-C80B858E258A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B465E55-007B-48C9-9E95-B8E3EBF760B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12300" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9060" firstSheet="4" activeTab="7" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
   </bookViews>
   <sheets>
     <sheet name="view 1 (rates up)" sheetId="1" r:id="rId1"/>
@@ -1601,10 +1601,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D192AB-C94F-4991-A9BC-7033E27831F6}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C25" sqref="C25"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1663,7 +1663,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="10">
-        <v>0.25</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
@@ -1678,7 +1678,7 @@
         <f t="shared" ref="I2" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
-        <v xml:space="preserve">μ_Germany 10-Year Government Bond Yield (p.a.) &gt; 0,25 </v>
+        <v xml:space="preserve">μ_Germany 10-Year Government Bond Yield (p.a.) &gt; 0,025 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1758,7 +1758,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C25" sqref="C25"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1817,7 +1817,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="10">
-        <v>-0.25</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
@@ -1832,7 +1832,7 @@
         <f t="shared" ref="I2" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
-        <v xml:space="preserve">μ_EUR Government Bonds (p.a.) &lt; -0,25 </v>
+        <v xml:space="preserve">μ_EUR Government Bonds (p.a.) &lt; -0,025 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1969,7 +1969,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="10">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
@@ -1984,7 +1984,7 @@
         <f t="shared" ref="I2" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
-        <v xml:space="preserve">μ_Global Equities (p.a.) &gt; 0,1 </v>
+        <v xml:space="preserve">μ_Global Equities (p.a.) &gt; 0,01 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2109,7 +2109,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
@@ -2124,7 +2124,7 @@
         <f t="shared" ref="I2" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
-        <v xml:space="preserve">μ_Global Equities (p.a.) &lt; -0,1 </v>
+        <v xml:space="preserve">μ_Global Equities (p.a.) &lt; -0,01 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2249,7 +2249,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="10">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
@@ -2264,7 +2264,7 @@
         <f t="shared" ref="I2" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
-        <v xml:space="preserve">μ_Eurozone Core Inflation (p.a.) &gt; 0,01 </v>
+        <v xml:space="preserve">μ_Eurozone Core Inflation (p.a.) &gt; 0,001 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2389,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="10">
-        <v>-0.01</v>
+        <v>-1E-3</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
@@ -2404,7 +2404,7 @@
         <f t="shared" ref="I2" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
-        <v xml:space="preserve">μ_Eurozone Core Inflation (p.a.) &lt; -0,01 </v>
+        <v xml:space="preserve">μ_Eurozone Core Inflation (p.a.) &lt; -0,001 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2529,7 +2529,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="10">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
@@ -2544,7 +2544,7 @@
         <f t="shared" ref="I2" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
-        <v xml:space="preserve">μ_iVol US Equities (p.a.) &gt; 0,1 </v>
+        <v xml:space="preserve">μ_iVol US Equities (p.a.) &gt; 0,01 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2609,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6705A1-063F-4EAE-B086-A9A750C92524}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2669,7 +2669,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
@@ -2684,7 +2684,7 @@
         <f t="shared" ref="I2" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
 &amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
-        <v xml:space="preserve">μ_iVol US Equities (p.a.) &lt; -0,1 </v>
+        <v xml:space="preserve">μ_iVol US Equities (p.a.) &lt; -0,01 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>